<commit_message>
updated functions to help with non-numeric data
</commit_message>
<xml_diff>
--- a/data/raw/sample_run_2019-03-01_CORRECTED.xlsx
+++ b/data/raw/sample_run_2019-03-01_CORRECTED.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\204.46.92.163\Public\Astoria Pacific nutrient runs\Steven Shivers Cyano\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Public\Astoria Pacific nutrient runs\Steven Shivers Cyano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBF8046-F6DC-42DE-B921-DD938BDF91B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A113819-EAF9-4283-A133-FE39CC0BA44D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="202">
   <si>
     <t>Run Name: sample_run_2019-03-01</t>
   </si>
@@ -721,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -747,9 +747,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -771,6 +768,12 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1112,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1143,33 +1146,33 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="13" t="s">
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="M5" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="12" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1704,11 +1707,11 @@
       <c r="K21" s="7">
         <v>0.505</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="9">
         <f>((100-H21)/100)*-100</f>
         <v>-0.63700000000000045</v>
       </c>
-      <c r="M21" s="11"/>
+      <c r="M21" s="10"/>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
@@ -1744,8 +1747,8 @@
       <c r="K22" s="7">
         <v>5.8570000000000002</v>
       </c>
-      <c r="L22" s="11"/>
-      <c r="M22" s="10">
+      <c r="L22" s="10"/>
+      <c r="M22" s="9">
         <f>((6-K22)/6)*-100</f>
         <v>-2.3833333333333302</v>
       </c>
@@ -1782,8 +1785,8 @@
       <c r="K23" s="7">
         <v>0.33400000000000002</v>
       </c>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
@@ -1817,8 +1820,8 @@
       <c r="K24" s="7">
         <v>188.63900000000001</v>
       </c>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
@@ -1852,8 +1855,8 @@
       <c r="K25" s="7">
         <v>1.5669999999999999</v>
       </c>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
@@ -1887,8 +1890,8 @@
       <c r="K26" s="7">
         <v>0.21299999999999999</v>
       </c>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
@@ -1912,7 +1915,7 @@
       <c r="G27" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="18">
         <v>1.325</v>
       </c>
       <c r="I27" s="6">
@@ -1921,11 +1924,11 @@
       <c r="J27" s="6">
         <v>0</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="18">
         <v>0.503</v>
       </c>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
@@ -1949,7 +1952,7 @@
       <c r="G28" s="6">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="18">
         <v>34.225999999999999</v>
       </c>
       <c r="I28" s="6">
@@ -1958,11 +1961,11 @@
       <c r="J28" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="18">
         <v>1.105</v>
       </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
@@ -1986,7 +1989,7 @@
       <c r="G29" s="6">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="18">
         <v>35.168999999999997</v>
       </c>
       <c r="I29" s="6">
@@ -1995,11 +1998,11 @@
       <c r="J29" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="18">
         <v>1.206</v>
       </c>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
@@ -2023,7 +2026,7 @@
       <c r="G30" s="6">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="18">
         <v>34.655000000000001</v>
       </c>
       <c r="I30" s="6">
@@ -2032,11 +2035,11 @@
       <c r="J30" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="18">
         <v>1.1930000000000001</v>
       </c>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
@@ -2060,7 +2063,7 @@
       <c r="G31" s="6">
         <v>0.14599999999999999</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="18">
         <v>62.665999999999997</v>
       </c>
       <c r="I31" s="6">
@@ -2069,11 +2072,11 @@
       <c r="J31" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K31" s="7">
+      <c r="K31" s="18">
         <v>1.2430000000000001</v>
       </c>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
@@ -2097,7 +2100,7 @@
       <c r="G32" s="6">
         <v>0.14899999999999999</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="18">
         <v>64.034000000000006</v>
       </c>
       <c r="I32" s="6">
@@ -2106,11 +2109,11 @@
       <c r="J32" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="18">
         <v>1.35</v>
       </c>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
@@ -2134,7 +2137,7 @@
       <c r="G33" s="6">
         <v>0.17100000000000001</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="18">
         <v>73.825999999999993</v>
       </c>
       <c r="I33" s="6">
@@ -2143,11 +2146,11 @@
       <c r="J33" s="6">
         <v>2E-3</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="18">
         <v>1.88</v>
       </c>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
@@ -2171,7 +2174,7 @@
       <c r="G34" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="18">
         <v>29.305</v>
       </c>
       <c r="I34" s="6">
@@ -2180,11 +2183,11 @@
       <c r="J34" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K34" s="7">
+      <c r="K34" s="18">
         <v>1.083</v>
       </c>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
@@ -2208,7 +2211,7 @@
       <c r="G35" s="6">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="18">
         <v>26.643999999999998</v>
       </c>
       <c r="I35" s="6">
@@ -2217,11 +2220,11 @@
       <c r="J35" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K35" s="7">
+      <c r="K35" s="18">
         <v>1.0389999999999999</v>
       </c>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
@@ -2245,7 +2248,7 @@
       <c r="G36" s="6">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="18">
         <v>26.939</v>
       </c>
       <c r="I36" s="6">
@@ -2254,24 +2257,24 @@
       <c r="J36" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K36" s="7">
+      <c r="K36" s="18">
         <v>1.1970000000000001</v>
       </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="12">
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="11">
         <f>((H36-H39)/((H36+H39)/2))*100</f>
         <v>3.1177546134851433</v>
       </c>
-      <c r="O36" s="12">
+      <c r="O36" s="11">
         <f>((K36-K39)/((K36+K39)/2))*100</f>
         <v>4.527979495941918</v>
       </c>
-      <c r="P36" s="17">
+      <c r="P36" s="16">
         <f>AVERAGE(H36,H39)</f>
         <v>26.525500000000001</v>
       </c>
-      <c r="Q36" s="17">
+      <c r="Q36" s="16">
         <f>AVERAGE(K36,K39)</f>
         <v>1.1705000000000001</v>
       </c>
@@ -2364,7 +2367,7 @@
       <c r="G39" s="6">
         <v>6.2E-2</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="18">
         <v>26.111999999999998</v>
       </c>
       <c r="I39" s="6">
@@ -2373,7 +2376,7 @@
       <c r="J39" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K39" s="7">
+      <c r="K39" s="18">
         <v>1.1439999999999999</v>
       </c>
     </row>
@@ -2399,7 +2402,7 @@
       <c r="G40" s="6">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="18">
         <v>30.062000000000001</v>
       </c>
       <c r="I40" s="6">
@@ -2408,7 +2411,7 @@
       <c r="J40" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K40" s="7">
+      <c r="K40" s="18">
         <v>1.403</v>
       </c>
     </row>
@@ -2434,7 +2437,7 @@
       <c r="G41" s="6">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="18">
         <v>30.876999999999999</v>
       </c>
       <c r="I41" s="6">
@@ -2443,7 +2446,7 @@
       <c r="J41" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K41" s="7">
+      <c r="K41" s="18">
         <v>1.4079999999999999</v>
       </c>
     </row>
@@ -2469,7 +2472,7 @@
       <c r="G42" s="6">
         <v>0.01</v>
       </c>
-      <c r="H42" s="7">
+      <c r="H42" s="18">
         <v>3.258</v>
       </c>
       <c r="I42" s="6">
@@ -2478,7 +2481,7 @@
       <c r="J42" s="6">
         <v>0</v>
       </c>
-      <c r="K42" s="7">
+      <c r="K42" s="18">
         <v>0.61</v>
       </c>
     </row>
@@ -2504,7 +2507,7 @@
       <c r="G43" s="6">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="H43" s="7">
+      <c r="H43" s="18">
         <v>26.655000000000001</v>
       </c>
       <c r="I43" s="6">
@@ -2513,7 +2516,7 @@
       <c r="J43" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K43" s="7">
+      <c r="K43" s="18">
         <v>0.91800000000000004</v>
       </c>
     </row>
@@ -2551,11 +2554,11 @@
       <c r="K44" s="7">
         <v>0.69499999999999995</v>
       </c>
-      <c r="L44" s="10">
+      <c r="L44" s="9">
         <f>((100-H44)/100)*-100</f>
         <v>1.3700000000000045</v>
       </c>
-      <c r="M44" s="11"/>
+      <c r="M44" s="10"/>
     </row>
     <row r="45" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
@@ -2591,8 +2594,8 @@
       <c r="K45" s="7">
         <v>6.157</v>
       </c>
-      <c r="L45" s="11"/>
-      <c r="M45" s="10">
+      <c r="L45" s="10"/>
+      <c r="M45" s="9">
         <f>((6-K45)/6)*-100</f>
         <v>2.6166666666666671</v>
       </c>
@@ -2619,7 +2622,7 @@
       <c r="G46" s="6">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="H46" s="7">
+      <c r="H46" s="18">
         <v>26.751999999999999</v>
       </c>
       <c r="I46" s="6">
@@ -2628,7 +2631,7 @@
       <c r="J46" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K46" s="7">
+      <c r="K46" s="18">
         <v>1.1160000000000001</v>
       </c>
     </row>
@@ -2654,7 +2657,7 @@
       <c r="G47" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="H47" s="7">
+      <c r="H47" s="18">
         <v>28.364000000000001</v>
       </c>
       <c r="I47" s="6">
@@ -2663,7 +2666,7 @@
       <c r="J47" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K47" s="7">
+      <c r="K47" s="18">
         <v>0.90300000000000002</v>
       </c>
     </row>
@@ -2689,7 +2692,7 @@
       <c r="G48" s="6">
         <v>0.159</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H48" s="18">
         <v>68.313000000000002</v>
       </c>
       <c r="I48" s="6">
@@ -2698,7 +2701,7 @@
       <c r="J48" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K48" s="7">
+      <c r="K48" s="18">
         <v>1.3129999999999999</v>
       </c>
     </row>
@@ -2724,7 +2727,7 @@
       <c r="G49" s="6">
         <v>0.16300000000000001</v>
       </c>
-      <c r="H49" s="7">
+      <c r="H49" s="18">
         <v>70.323999999999998</v>
       </c>
       <c r="I49" s="6">
@@ -2733,7 +2736,7 @@
       <c r="J49" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K49" s="7">
+      <c r="K49" s="18">
         <v>1.3280000000000001</v>
       </c>
     </row>
@@ -2759,7 +2762,7 @@
       <c r="G50" s="6">
         <v>0.17</v>
       </c>
-      <c r="H50" s="7">
+      <c r="H50" s="18">
         <v>73.403999999999996</v>
       </c>
       <c r="I50" s="6">
@@ -2768,7 +2771,7 @@
       <c r="J50" s="6">
         <v>2E-3</v>
       </c>
-      <c r="K50" s="7">
+      <c r="K50" s="18">
         <v>1.738</v>
       </c>
     </row>
@@ -2860,7 +2863,7 @@
       <c r="G53" s="6">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="H53" s="7">
+      <c r="H53" s="18">
         <v>27.436</v>
       </c>
       <c r="I53" s="6">
@@ -2869,22 +2872,22 @@
       <c r="J53" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K53" s="15">
+      <c r="K53" s="14">
         <v>0.96599999999999997</v>
       </c>
-      <c r="N53" s="12">
+      <c r="N53" s="11">
         <f>((H53-H54)/((H53+H54)/2))*100</f>
         <v>-2.8456453003736764</v>
       </c>
-      <c r="O53" s="14">
+      <c r="O53" s="13">
         <f>((K53-K54)/((K53+K54)/2))*100</f>
         <v>22.837370242214526</v>
       </c>
-      <c r="P53" s="17">
+      <c r="P53" s="16">
         <f>AVERAGE(H53,H54)</f>
         <v>27.832000000000001</v>
       </c>
-      <c r="Q53" s="16">
+      <c r="Q53" s="15">
         <f>AVERAGE(K53,K54)</f>
         <v>0.86699999999999999</v>
       </c>
@@ -2911,7 +2914,7 @@
       <c r="G54" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="H54" s="7">
+      <c r="H54" s="18">
         <v>28.228000000000002</v>
       </c>
       <c r="I54" s="6">
@@ -2920,7 +2923,7 @@
       <c r="J54" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K54" s="15">
+      <c r="K54" s="14">
         <v>0.76800000000000002</v>
       </c>
     </row>
@@ -2946,7 +2949,7 @@
       <c r="G55" s="6">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="H55" s="7">
+      <c r="H55" s="18">
         <v>28.501999999999999</v>
       </c>
       <c r="I55" s="6">
@@ -2955,7 +2958,7 @@
       <c r="J55" s="6">
         <v>0</v>
       </c>
-      <c r="K55" s="7">
+      <c r="K55" s="18">
         <v>0.51200000000000001</v>
       </c>
     </row>
@@ -2981,7 +2984,7 @@
       <c r="G56" s="6">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="H56" s="7">
+      <c r="H56" s="18">
         <v>30.074000000000002</v>
       </c>
       <c r="I56" s="6">
@@ -2990,7 +2993,7 @@
       <c r="J56" s="6">
         <v>0</v>
       </c>
-      <c r="K56" s="7">
+      <c r="K56" s="18">
         <v>0.36</v>
       </c>
     </row>
@@ -3016,7 +3019,7 @@
       <c r="G57" s="6">
         <v>0.153</v>
       </c>
-      <c r="H57" s="7">
+      <c r="H57" s="18">
         <v>66.040999999999997</v>
       </c>
       <c r="I57" s="6">
@@ -3025,7 +3028,7 @@
       <c r="J57" s="6">
         <v>0</v>
       </c>
-      <c r="K57" s="7">
+      <c r="K57" s="18">
         <v>0.13900000000000001</v>
       </c>
     </row>
@@ -3051,7 +3054,7 @@
       <c r="G58" s="6">
         <v>0.16900000000000001</v>
       </c>
-      <c r="H58" s="7">
+      <c r="H58" s="18">
         <v>72.899000000000001</v>
       </c>
       <c r="I58" s="6">
@@ -3060,7 +3063,7 @@
       <c r="J58" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K58" s="7">
+      <c r="K58" s="18">
         <v>3.4220000000000002</v>
       </c>
     </row>
@@ -3086,7 +3089,7 @@
       <c r="G59" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="H59" s="15">
+      <c r="H59" s="14">
         <v>7.2060000000000004</v>
       </c>
       <c r="I59" s="6">
@@ -3095,7 +3098,7 @@
       <c r="J59" s="6">
         <v>-1E-3</v>
       </c>
-      <c r="K59" s="15">
+      <c r="K59" s="14">
         <v>-1.147</v>
       </c>
     </row>
@@ -3121,7 +3124,7 @@
       <c r="G60" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H60" s="15">
+      <c r="H60" s="14">
         <v>0.46899999999999997</v>
       </c>
       <c r="I60" s="6">
@@ -3130,7 +3133,7 @@
       <c r="J60" s="6">
         <v>-2E-3</v>
       </c>
-      <c r="K60" s="15">
+      <c r="K60" s="14">
         <v>-2.19</v>
       </c>
     </row>
@@ -3156,7 +3159,7 @@
       <c r="G61" s="6">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="H61" s="15">
+      <c r="H61" s="14">
         <v>22.084</v>
       </c>
       <c r="I61" s="6">
@@ -3165,7 +3168,7 @@
       <c r="J61" s="6">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="K61" s="15">
+      <c r="K61" s="14">
         <v>41.595999999999997</v>
       </c>
     </row>
@@ -3191,7 +3194,7 @@
       <c r="G62" s="6">
         <v>0.124</v>
       </c>
-      <c r="H62" s="15">
+      <c r="H62" s="14">
         <v>53.088000000000001</v>
       </c>
       <c r="I62" s="6">
@@ -3200,7 +3203,7 @@
       <c r="J62" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="K62" s="15">
+      <c r="K62" s="14">
         <v>11.749000000000001</v>
       </c>
     </row>
@@ -3304,11 +3307,11 @@
       <c r="K65" s="7">
         <v>0.68</v>
       </c>
-      <c r="L65" s="10">
+      <c r="L65" s="9">
         <f>((100-H65)/100)*-100</f>
         <v>0.25400000000000489</v>
       </c>
-      <c r="M65" s="11"/>
+      <c r="M65" s="10"/>
     </row>
     <row r="66" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
@@ -3344,8 +3347,8 @@
       <c r="K66" s="7">
         <v>6.0149999999999997</v>
       </c>
-      <c r="L66" s="11"/>
-      <c r="M66" s="10">
+      <c r="L66" s="10"/>
+      <c r="M66" s="9">
         <f>((6-K66)/6)*-100</f>
         <v>0.24999999999999467</v>
       </c>
@@ -3372,7 +3375,7 @@
       <c r="G67" s="6">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="H67" s="7">
+      <c r="H67" s="18">
         <v>29.067</v>
       </c>
       <c r="I67" s="6">
@@ -3381,7 +3384,7 @@
       <c r="J67" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K67" s="7">
+      <c r="K67" s="14">
         <v>1.1299999999999999</v>
       </c>
     </row>
@@ -3407,7 +3410,7 @@
       <c r="G68" s="6">
         <v>0.15</v>
       </c>
-      <c r="H68" s="7">
+      <c r="H68" s="18">
         <v>64.432000000000002</v>
       </c>
       <c r="I68" s="6">
@@ -3416,22 +3419,22 @@
       <c r="J68" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K68" s="7">
+      <c r="K68" s="14">
         <v>1.2210000000000001</v>
       </c>
-      <c r="N68" s="12">
+      <c r="N68" s="11">
         <f>((H68-H69)/((H68+H69)/2))*100</f>
         <v>-2.396743005666008</v>
       </c>
-      <c r="O68" s="12">
+      <c r="O68" s="11">
         <f>((K68-K69)/((K68+K69)/2))*100</f>
         <v>2.8239202657807332</v>
       </c>
-      <c r="P68" s="17">
+      <c r="P68" s="16">
         <f>AVERAGE(H68,H69)</f>
         <v>65.21350000000001</v>
       </c>
-      <c r="Q68" s="17">
+      <c r="Q68" s="16">
         <f>AVERAGE(K68,K69)</f>
         <v>1.2040000000000002</v>
       </c>
@@ -3458,7 +3461,7 @@
       <c r="G69" s="6">
         <v>0.153</v>
       </c>
-      <c r="H69" s="7">
+      <c r="H69" s="18">
         <v>65.995000000000005</v>
       </c>
       <c r="I69" s="6">
@@ -3467,7 +3470,7 @@
       <c r="J69" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K69" s="7">
+      <c r="K69" s="14">
         <v>1.1870000000000001</v>
       </c>
     </row>
@@ -3493,7 +3496,7 @@
       <c r="G70" s="6">
         <v>0.154</v>
       </c>
-      <c r="H70" s="7">
+      <c r="H70" s="18">
         <v>66.197000000000003</v>
       </c>
       <c r="I70" s="6">
@@ -3502,7 +3505,7 @@
       <c r="J70" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K70" s="7">
+      <c r="K70" s="14">
         <v>1.0429999999999999</v>
       </c>
     </row>
@@ -3528,7 +3531,7 @@
       <c r="G71" s="6">
         <v>0.14899999999999999</v>
       </c>
-      <c r="H71" s="7">
+      <c r="H71" s="18">
         <v>64.275999999999996</v>
       </c>
       <c r="I71" s="6">
@@ -3537,7 +3540,7 @@
       <c r="J71" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K71" s="7">
+      <c r="K71" s="14">
         <v>1.052</v>
       </c>
     </row>
@@ -3563,7 +3566,7 @@
       <c r="G72" s="6">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="H72" s="7">
+      <c r="H72" s="18">
         <v>28.376000000000001</v>
       </c>
       <c r="I72" s="6">
@@ -3572,7 +3575,7 @@
       <c r="J72" s="6">
         <v>0</v>
       </c>
-      <c r="K72" s="7">
+      <c r="K72" s="14">
         <v>0.55700000000000005</v>
       </c>
     </row>
@@ -3598,7 +3601,7 @@
       <c r="G73" s="6">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="H73" s="7">
+      <c r="H73" s="18">
         <v>27.661000000000001</v>
       </c>
       <c r="I73" s="6">
@@ -3607,7 +3610,7 @@
       <c r="J73" s="6">
         <v>0</v>
       </c>
-      <c r="K73" s="7">
+      <c r="K73" s="14">
         <v>0.61399999999999999</v>
       </c>
     </row>
@@ -3633,7 +3636,7 @@
       <c r="G74" s="6">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="H74" s="7">
+      <c r="H74" s="18">
         <v>30.004000000000001</v>
       </c>
       <c r="I74" s="6">
@@ -3642,7 +3645,7 @@
       <c r="J74" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K74" s="7">
+      <c r="K74" s="14">
         <v>0.80600000000000005</v>
       </c>
     </row>
@@ -3668,7 +3671,7 @@
       <c r="G75" s="6">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H75" s="7">
+      <c r="H75" s="18">
         <v>35.899000000000001</v>
       </c>
       <c r="I75" s="6">
@@ -3677,7 +3680,7 @@
       <c r="J75" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K75" s="7">
+      <c r="K75" s="14">
         <v>1.1759999999999999</v>
       </c>
     </row>
@@ -3703,7 +3706,7 @@
       <c r="G76" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="H76" s="7">
+      <c r="H76" s="18">
         <v>4.1550000000000002</v>
       </c>
       <c r="I76" s="6">
@@ -3712,7 +3715,7 @@
       <c r="J76" s="6">
         <v>0</v>
       </c>
-      <c r="K76" s="7">
+      <c r="K76" s="14">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -3804,7 +3807,7 @@
       <c r="G79" s="6">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="H79" s="7">
+      <c r="H79" s="18">
         <v>36.35</v>
       </c>
       <c r="I79" s="6">
@@ -3813,7 +3816,7 @@
       <c r="J79" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K79" s="7">
+      <c r="K79" s="18">
         <v>1.2889999999999999</v>
       </c>
     </row>
@@ -3839,7 +3842,7 @@
       <c r="G80" s="6">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="H80" s="7">
+      <c r="H80" s="18">
         <v>37.313000000000002</v>
       </c>
       <c r="I80" s="6">
@@ -3848,7 +3851,7 @@
       <c r="J80" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K80" s="7">
+      <c r="K80" s="18">
         <v>1.2370000000000001</v>
       </c>
     </row>
@@ -3874,7 +3877,7 @@
       <c r="G81" s="6">
         <v>0.17399999999999999</v>
       </c>
-      <c r="H81" s="7">
+      <c r="H81" s="18">
         <v>75.161000000000001</v>
       </c>
       <c r="I81" s="6">
@@ -3883,22 +3886,22 @@
       <c r="J81" s="6">
         <v>2E-3</v>
       </c>
-      <c r="K81" s="7">
+      <c r="K81" s="18">
         <v>2.0510000000000002</v>
       </c>
-      <c r="N81" s="12">
+      <c r="N81" s="11">
         <f>((H81-H82)/((H81+H82)/2))*100</f>
         <v>-2.3275385950608793</v>
       </c>
-      <c r="O81" s="12">
+      <c r="O81" s="11">
         <f>((K81-K82)/((K81+K82)/2))*100</f>
         <v>3.0190546894333163</v>
       </c>
-      <c r="P81" s="17">
+      <c r="P81" s="16">
         <f>AVERAGE(H81,H82)</f>
         <v>76.045999999999992</v>
       </c>
-      <c r="Q81" s="17">
+      <c r="Q81" s="16">
         <f>AVERAGE(K81,K82)</f>
         <v>2.0205000000000002</v>
       </c>
@@ -3925,7 +3928,7 @@
       <c r="G82" s="6">
         <v>0.17799999999999999</v>
       </c>
-      <c r="H82" s="7">
+      <c r="H82" s="18">
         <v>76.930999999999997</v>
       </c>
       <c r="I82" s="6">
@@ -3934,7 +3937,7 @@
       <c r="J82" s="6">
         <v>2E-3</v>
       </c>
-      <c r="K82" s="7">
+      <c r="K82" s="18">
         <v>1.99</v>
       </c>
     </row>
@@ -3960,7 +3963,7 @@
       <c r="G83" s="6">
         <v>0.184</v>
       </c>
-      <c r="H83" s="7">
+      <c r="H83" s="18">
         <v>79.257000000000005</v>
       </c>
       <c r="I83" s="6">
@@ -3969,7 +3972,7 @@
       <c r="J83" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K83" s="7">
+      <c r="K83" s="18">
         <v>1.532</v>
       </c>
     </row>
@@ -4007,11 +4010,11 @@
       <c r="K84" s="7">
         <v>0.84399999999999997</v>
       </c>
-      <c r="L84" s="10">
+      <c r="L84" s="9">
         <f>((100-H84)/100)*-100</f>
         <v>2.9539999999999935</v>
       </c>
-      <c r="M84" s="11"/>
+      <c r="M84" s="10"/>
     </row>
     <row r="85" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
@@ -4047,8 +4050,8 @@
       <c r="K85" s="7">
         <v>6.33</v>
       </c>
-      <c r="L85" s="11"/>
-      <c r="M85" s="10">
+      <c r="L85" s="10"/>
+      <c r="M85" s="9">
         <f>((6-K85)/6)*-100</f>
         <v>5.5000000000000018</v>
       </c>
@@ -4075,7 +4078,7 @@
       <c r="G86" s="6">
         <v>0.17199999999999999</v>
       </c>
-      <c r="H86" s="7">
+      <c r="H86" s="18">
         <v>74.302000000000007</v>
       </c>
       <c r="I86" s="6">
@@ -4084,7 +4087,7 @@
       <c r="J86" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K86" s="7">
+      <c r="K86" s="18">
         <v>1.4630000000000001</v>
       </c>
     </row>
@@ -4110,7 +4113,7 @@
       <c r="G87" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="H87" s="7">
+      <c r="H87" s="18">
         <v>28.039000000000001</v>
       </c>
       <c r="I87" s="6">
@@ -4119,7 +4122,7 @@
       <c r="J87" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K87" s="7">
+      <c r="K87" s="18">
         <v>0.97499999999999998</v>
       </c>
     </row>
@@ -4145,7 +4148,7 @@
       <c r="G88" s="6">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="H88" s="7">
+      <c r="H88" s="18">
         <v>27.443999999999999</v>
       </c>
       <c r="I88" s="6">
@@ -4154,7 +4157,7 @@
       <c r="J88" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K88" s="7">
+      <c r="K88" s="18">
         <v>1.33</v>
       </c>
     </row>
@@ -4180,7 +4183,7 @@
       <c r="G89" s="6">
         <v>6.2E-2</v>
       </c>
-      <c r="H89" s="7">
+      <c r="H89" s="18">
         <v>25.928000000000001</v>
       </c>
       <c r="I89" s="6">
@@ -4189,7 +4192,7 @@
       <c r="J89" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K89" s="7">
+      <c r="K89" s="18">
         <v>0.98</v>
       </c>
     </row>
@@ -4215,7 +4218,7 @@
       <c r="G90" s="6">
         <v>0.01</v>
       </c>
-      <c r="H90" s="7">
+      <c r="H90" s="18">
         <v>3.2069999999999999</v>
       </c>
       <c r="I90" s="6">
@@ -4224,7 +4227,7 @@
       <c r="J90" s="6">
         <v>0</v>
       </c>
-      <c r="K90" s="7">
+      <c r="K90" s="18">
         <v>0.66100000000000003</v>
       </c>
     </row>
@@ -4316,7 +4319,7 @@
       <c r="G93" s="6">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="H93" s="7">
+      <c r="H93" s="18">
         <v>28.835000000000001</v>
       </c>
       <c r="I93" s="6">
@@ -4325,7 +4328,7 @@
       <c r="J93" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K93" s="7">
+      <c r="K93" s="18">
         <v>1.4570000000000001</v>
       </c>
     </row>
@@ -4340,7 +4343,7 @@
         <v>152</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>17</v>
@@ -4351,7 +4354,7 @@
       <c r="G94" s="6">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="H94" s="7">
+      <c r="H94" s="18">
         <v>29.861000000000001</v>
       </c>
       <c r="I94" s="6">
@@ -4360,7 +4363,7 @@
       <c r="J94" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K94" s="7">
+      <c r="K94" s="18">
         <v>1.389</v>
       </c>
     </row>
@@ -4375,7 +4378,7 @@
         <v>154</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>17</v>
@@ -4386,7 +4389,7 @@
       <c r="G95" s="6">
         <v>0.159</v>
       </c>
-      <c r="H95" s="7">
+      <c r="H95" s="18">
         <v>68.438000000000002</v>
       </c>
       <c r="I95" s="6">
@@ -4395,7 +4398,7 @@
       <c r="J95" s="6">
         <v>2E-3</v>
       </c>
-      <c r="K95" s="7">
+      <c r="K95" s="18">
         <v>1.706</v>
       </c>
     </row>
@@ -4499,11 +4502,11 @@
       <c r="K98" s="7">
         <v>0.87</v>
       </c>
-      <c r="L98" s="10">
+      <c r="L98" s="9">
         <f>((100-H98)/100)*-100</f>
         <v>7.9999999999955662E-3</v>
       </c>
-      <c r="M98" s="11"/>
+      <c r="M98" s="10"/>
     </row>
     <row r="99" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
@@ -4539,8 +4542,8 @@
       <c r="K99" s="7">
         <v>6.3840000000000003</v>
       </c>
-      <c r="L99" s="11"/>
-      <c r="M99" s="10">
+      <c r="L99" s="10"/>
+      <c r="M99" s="9">
         <f>((6-K99)/6)*-100</f>
         <v>6.4000000000000057</v>
       </c>

</xml_diff>